<commit_message>
OW-981,OW-982, added the tests
</commit_message>
<xml_diff>
--- a/test/testIntegerRatio/integerRatioPerformance1.xlsx
+++ b/test/testIntegerRatio/integerRatioPerformance1.xlsx
@@ -53,6 +53,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,7 +101,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -113,6 +116,12 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -423,12 +432,14 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A1:G13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -467,10 +478,10 @@
       <c r="D2" s="3">
         <v>10.579999999999901</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <v>378.478351910073</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="6">
         <v>0.84460594003126999</v>
       </c>
       <c r="G2" s="3">
@@ -490,10 +501,10 @@
       <c r="D3" s="3">
         <v>12.6199999999999</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="6">
         <v>466.25626146401902</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="6">
         <v>0.84177410993504198</v>
       </c>
       <c r="G3" s="3">
@@ -513,10 +524,10 @@
       <c r="D4" s="3">
         <v>10.399999999999601</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>396.31642654068901</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="6">
         <v>0.85064558721997996</v>
       </c>
       <c r="G4" s="3">
@@ -536,10 +547,10 @@
       <c r="D5" s="3">
         <v>10.359999999999699</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>396.31636911914899</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="6">
         <v>0.850645605489882</v>
       </c>
       <c r="G5" s="3">
@@ -559,10 +570,10 @@
       <c r="D6" s="3">
         <v>10.4499999999998</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>384.47808345966303</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>0.80933039324987399</v>
       </c>
       <c r="G6" s="3">
@@ -582,10 +593,10 @@
       <c r="D7" s="3">
         <v>11.5500000000002</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>396.31748334253001</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>0.81459178088626305</v>
       </c>
       <c r="G7" s="3">
@@ -605,10 +616,10 @@
       <c r="D8" s="3">
         <v>10.3600000000006</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>396.316474466344</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="6">
         <v>0.81459223512048395</v>
       </c>
       <c r="G8" s="3">
@@ -628,10 +639,10 @@
       <c r="D9" s="3">
         <v>10.4499999999998</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="6">
         <v>396.31636938246601</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="6">
         <v>0.81459227602136097</v>
       </c>
       <c r="G9" s="3">
@@ -651,10 +662,10 @@
       <c r="D10" s="5">
         <v>10.3099999999995</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="7">
         <v>378.62044197039597</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="7">
         <v>0.63957470752908196</v>
       </c>
       <c r="G10" s="5">
@@ -674,10 +685,10 @@
       <c r="D11" s="3">
         <v>11.590000000000099</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="6">
         <v>466.33974025408799</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="6">
         <v>0.631559021683055</v>
       </c>
       <c r="G11" s="3">
@@ -697,10 +708,10 @@
       <c r="D12" s="3">
         <v>10.3099999999995</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="6">
         <v>396.31642709956901</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="6">
         <v>0.65342095339911699</v>
       </c>
       <c r="G12" s="3">
@@ -720,10 +731,10 @@
       <c r="D13" s="3">
         <v>10.329999999999901</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="6">
         <v>396.31636754091801</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="6">
         <v>0.65342099732186998</v>
       </c>
       <c r="G13" s="3">

</xml_diff>